<commit_message>
Moved OSU research notebooks to the osu_research folder
</commit_message>
<xml_diff>
--- a/data/xlsx/anova290_df_Apr24_Final.xlsx
+++ b/data/xlsx/anova290_df_Apr24_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaveBabbitt\Documents\GitHub\itm-analysis-reporting\data\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dway\Documents\Work Folder\Danforth Grant\Darpa Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8411D3-B2E2-4B25-B89E-FFDC83FD2954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9D80888-C8D8-43D4-B456-CE2B6152D601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7560" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21405" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anova290_df_Apr24_Final" sheetId="1" r:id="rId1"/>
@@ -4416,31 +4416,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.09765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4481,7 +4469,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -4522,7 +4510,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -4563,7 +4551,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -4604,7 +4592,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -4645,7 +4633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -4686,7 +4674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -4727,7 +4715,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -4768,7 +4756,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -4809,7 +4797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -4850,7 +4838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -4891,7 +4879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -4932,7 +4920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -4973,7 +4961,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -5014,7 +5002,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -5055,7 +5043,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -5096,7 +5084,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -5137,7 +5125,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -5178,7 +5166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -5219,7 +5207,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -5260,7 +5248,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -5301,7 +5289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>96</v>
       </c>
@@ -5342,7 +5330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>100</v>
       </c>
@@ -5383,7 +5371,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -5424,7 +5412,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -5465,7 +5453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -5506,7 +5494,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>117</v>
       </c>
@@ -5547,7 +5535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>121</v>
       </c>
@@ -5588,7 +5576,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>125</v>
       </c>
@@ -5629,7 +5617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>129</v>
       </c>
@@ -5670,7 +5658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>133</v>
       </c>
@@ -5711,7 +5699,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>137</v>
       </c>
@@ -5752,7 +5740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>141</v>
       </c>
@@ -5793,7 +5781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -5834,7 +5822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>149</v>
       </c>
@@ -5875,7 +5863,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>153</v>
       </c>
@@ -5916,7 +5904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -5957,7 +5945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>161</v>
       </c>
@@ -5998,7 +5986,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -6039,7 +6027,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>169</v>
       </c>
@@ -6080,7 +6068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>173</v>
       </c>
@@ -6121,7 +6109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>177</v>
       </c>
@@ -6162,7 +6150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>181</v>
       </c>
@@ -6203,7 +6191,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>185</v>
       </c>
@@ -6244,7 +6232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>189</v>
       </c>
@@ -6285,7 +6273,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>193</v>
       </c>
@@ -6326,7 +6314,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>197</v>
       </c>
@@ -6367,7 +6355,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>201</v>
       </c>
@@ -6408,7 +6396,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>205</v>
       </c>
@@ -6449,7 +6437,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>209</v>
       </c>
@@ -6490,7 +6478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>214</v>
       </c>
@@ -6531,7 +6519,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>218</v>
       </c>
@@ -6572,7 +6560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -6613,7 +6601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>227</v>
       </c>
@@ -6654,7 +6642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>231</v>
       </c>
@@ -6695,7 +6683,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>235</v>
       </c>
@@ -6736,7 +6724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>239</v>
       </c>
@@ -6777,7 +6765,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>243</v>
       </c>
@@ -6818,7 +6806,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>247</v>
       </c>
@@ -6859,7 +6847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>251</v>
       </c>
@@ -6900,7 +6888,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>255</v>
       </c>
@@ -6941,7 +6929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>259</v>
       </c>
@@ -6982,7 +6970,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>263</v>
       </c>
@@ -7023,7 +7011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>267</v>
       </c>
@@ -7064,7 +7052,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>271</v>
       </c>
@@ -7105,7 +7093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>275</v>
       </c>
@@ -7146,7 +7134,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>279</v>
       </c>
@@ -7187,7 +7175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>283</v>
       </c>
@@ -7228,7 +7216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>288</v>
       </c>
@@ -7269,7 +7257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>292</v>
       </c>
@@ -7310,7 +7298,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>296</v>
       </c>
@@ -7351,7 +7339,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>300</v>
       </c>
@@ -7392,7 +7380,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>304</v>
       </c>
@@ -7433,7 +7421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>308</v>
       </c>
@@ -7474,7 +7462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>312</v>
       </c>
@@ -7515,7 +7503,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>316</v>
       </c>
@@ -7556,7 +7544,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>320</v>
       </c>
@@ -7597,7 +7585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>324</v>
       </c>
@@ -7638,7 +7626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>328</v>
       </c>
@@ -7679,7 +7667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>332</v>
       </c>
@@ -7720,7 +7708,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>336</v>
       </c>
@@ -7761,7 +7749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>340</v>
       </c>
@@ -7802,7 +7790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>344</v>
       </c>
@@ -7843,7 +7831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>348</v>
       </c>
@@ -7884,7 +7872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>352</v>
       </c>
@@ -7925,7 +7913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>356</v>
       </c>
@@ -7966,7 +7954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>360</v>
       </c>
@@ -8007,7 +7995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>364</v>
       </c>
@@ -8048,7 +8036,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>368</v>
       </c>
@@ -8089,7 +8077,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>372</v>
       </c>
@@ -8130,7 +8118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>376</v>
       </c>
@@ -8171,7 +8159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>380</v>
       </c>
@@ -8212,7 +8200,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>384</v>
       </c>
@@ -8253,7 +8241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>388</v>
       </c>
@@ -8294,7 +8282,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>392</v>
       </c>
@@ -8335,7 +8323,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>396</v>
       </c>
@@ -8376,7 +8364,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>400</v>
       </c>
@@ -8417,7 +8405,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>404</v>
       </c>
@@ -8458,7 +8446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>408</v>
       </c>
@@ -8499,7 +8487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>412</v>
       </c>
@@ -8540,7 +8528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>416</v>
       </c>
@@ -8581,7 +8569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>420</v>
       </c>
@@ -8622,7 +8610,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>424</v>
       </c>
@@ -8663,7 +8651,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>428</v>
       </c>
@@ -8704,7 +8692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>432</v>
       </c>
@@ -8745,7 +8733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>436</v>
       </c>
@@ -8786,7 +8774,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>440</v>
       </c>
@@ -8827,7 +8815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>444</v>
       </c>
@@ -8868,7 +8856,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>448</v>
       </c>
@@ -8909,7 +8897,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>452</v>
       </c>
@@ -8950,7 +8938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>456</v>
       </c>
@@ -8991,7 +8979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>460</v>
       </c>
@@ -9032,7 +9020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>464</v>
       </c>
@@ -9073,7 +9061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>468</v>
       </c>
@@ -9114,7 +9102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>472</v>
       </c>
@@ -9155,7 +9143,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>476</v>
       </c>
@@ -9196,7 +9184,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>480</v>
       </c>
@@ -9237,7 +9225,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>484</v>
       </c>
@@ -9278,7 +9266,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>488</v>
       </c>
@@ -9319,7 +9307,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>492</v>
       </c>
@@ -9360,7 +9348,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>496</v>
       </c>
@@ -9401,7 +9389,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>500</v>
       </c>
@@ -9442,7 +9430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>504</v>
       </c>
@@ -9483,7 +9471,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>508</v>
       </c>
@@ -9524,7 +9512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>512</v>
       </c>
@@ -9565,7 +9553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>516</v>
       </c>
@@ -9606,7 +9594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>520</v>
       </c>
@@ -9647,7 +9635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>524</v>
       </c>
@@ -9688,7 +9676,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>528</v>
       </c>
@@ -9729,7 +9717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>532</v>
       </c>
@@ -9770,7 +9758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>536</v>
       </c>
@@ -9811,7 +9799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>540</v>
       </c>
@@ -9852,7 +9840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>544</v>
       </c>
@@ -9893,7 +9881,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>548</v>
       </c>
@@ -9934,7 +9922,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>552</v>
       </c>
@@ -9975,7 +9963,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>556</v>
       </c>
@@ -10016,7 +10004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>560</v>
       </c>
@@ -10057,7 +10045,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>564</v>
       </c>
@@ -10098,7 +10086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>568</v>
       </c>
@@ -10139,7 +10127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>572</v>
       </c>
@@ -10180,7 +10168,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>576</v>
       </c>
@@ -10221,7 +10209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>580</v>
       </c>
@@ -10262,7 +10250,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>584</v>
       </c>
@@ -10303,7 +10291,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>588</v>
       </c>
@@ -10344,7 +10332,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>592</v>
       </c>
@@ -10385,7 +10373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>596</v>
       </c>
@@ -10426,7 +10414,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>600</v>
       </c>
@@ -10467,7 +10455,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>604</v>
       </c>
@@ -10508,7 +10496,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>608</v>
       </c>
@@ -10549,7 +10537,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>612</v>
       </c>
@@ -10590,7 +10578,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>616</v>
       </c>
@@ -10631,7 +10619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>620</v>
       </c>
@@ -10672,7 +10660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>624</v>
       </c>
@@ -10713,7 +10701,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>628</v>
       </c>
@@ -10754,7 +10742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>632</v>
       </c>
@@ -10795,7 +10783,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>636</v>
       </c>
@@ -10836,7 +10824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>640</v>
       </c>
@@ -10877,7 +10865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>644</v>
       </c>
@@ -10918,7 +10906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>648</v>
       </c>
@@ -10959,7 +10947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>652</v>
       </c>
@@ -11000,7 +10988,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>656</v>
       </c>
@@ -11041,7 +11029,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>660</v>
       </c>
@@ -11082,7 +11070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>664</v>
       </c>
@@ -11123,7 +11111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>668</v>
       </c>
@@ -11164,7 +11152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>672</v>
       </c>
@@ -11205,7 +11193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>676</v>
       </c>
@@ -11246,7 +11234,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>680</v>
       </c>
@@ -11287,7 +11275,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>684</v>
       </c>
@@ -11328,7 +11316,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>688</v>
       </c>
@@ -11369,7 +11357,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>692</v>
       </c>
@@ -11410,7 +11398,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>696</v>
       </c>
@@ -11451,7 +11439,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>700</v>
       </c>
@@ -11492,7 +11480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>704</v>
       </c>
@@ -11533,7 +11521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>708</v>
       </c>
@@ -11574,7 +11562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>712</v>
       </c>
@@ -11615,7 +11603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>716</v>
       </c>
@@ -11656,7 +11644,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>720</v>
       </c>
@@ -11697,7 +11685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>724</v>
       </c>
@@ -11738,7 +11726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>728</v>
       </c>
@@ -11779,7 +11767,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>732</v>
       </c>
@@ -11820,7 +11808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>736</v>
       </c>
@@ -11861,7 +11849,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>740</v>
       </c>
@@ -11902,7 +11890,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>744</v>
       </c>
@@ -11943,7 +11931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>748</v>
       </c>
@@ -11984,7 +11972,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>752</v>
       </c>
@@ -12025,7 +12013,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>756</v>
       </c>
@@ -12066,7 +12054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>760</v>
       </c>
@@ -12107,7 +12095,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>764</v>
       </c>
@@ -12148,7 +12136,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>768</v>
       </c>
@@ -12189,7 +12177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>772</v>
       </c>
@@ -12230,7 +12218,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>776</v>
       </c>
@@ -12271,7 +12259,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>780</v>
       </c>
@@ -12312,7 +12300,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>784</v>
       </c>
@@ -12353,7 +12341,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>788</v>
       </c>
@@ -12394,7 +12382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>792</v>
       </c>
@@ -12435,7 +12423,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>796</v>
       </c>
@@ -12476,7 +12464,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>800</v>
       </c>
@@ -12517,7 +12505,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>804</v>
       </c>
@@ -12558,7 +12546,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>808</v>
       </c>
@@ -12599,7 +12587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>812</v>
       </c>
@@ -12640,7 +12628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>816</v>
       </c>
@@ -12681,7 +12669,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>820</v>
       </c>
@@ -12722,7 +12710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>824</v>
       </c>
@@ -12763,7 +12751,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>828</v>
       </c>
@@ -12804,7 +12792,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>832</v>
       </c>
@@ -12845,7 +12833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>836</v>
       </c>
@@ -12886,7 +12874,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>840</v>
       </c>
@@ -12927,7 +12915,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>844</v>
       </c>
@@ -12968,7 +12956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>848</v>
       </c>
@@ -13009,7 +12997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>852</v>
       </c>
@@ -13050,7 +13038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>856</v>
       </c>
@@ -13091,7 +13079,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>860</v>
       </c>
@@ -13132,7 +13120,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>864</v>
       </c>
@@ -13173,7 +13161,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>868</v>
       </c>
@@ -13214,7 +13202,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>872</v>
       </c>
@@ -13255,7 +13243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>876</v>
       </c>
@@ -13296,7 +13284,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>880</v>
       </c>
@@ -13337,7 +13325,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>884</v>
       </c>
@@ -13378,7 +13366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>888</v>
       </c>
@@ -13419,7 +13407,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>892</v>
       </c>
@@ -13460,7 +13448,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>896</v>
       </c>
@@ -13501,7 +13489,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>900</v>
       </c>
@@ -13542,7 +13530,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>904</v>
       </c>
@@ -13583,7 +13571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>908</v>
       </c>
@@ -13624,7 +13612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>912</v>
       </c>
@@ -13665,7 +13653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>916</v>
       </c>
@@ -13706,7 +13694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>920</v>
       </c>
@@ -13747,7 +13735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>924</v>
       </c>
@@ -13788,7 +13776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>928</v>
       </c>
@@ -13829,7 +13817,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>932</v>
       </c>
@@ -13870,7 +13858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>936</v>
       </c>
@@ -13911,7 +13899,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>940</v>
       </c>
@@ -13952,7 +13940,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>944</v>
       </c>
@@ -13993,7 +13981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>948</v>
       </c>
@@ -14034,7 +14022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>952</v>
       </c>
@@ -14075,7 +14063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>956</v>
       </c>
@@ -14116,7 +14104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>960</v>
       </c>
@@ -14157,7 +14145,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>964</v>
       </c>
@@ -14198,7 +14186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>968</v>
       </c>
@@ -14239,7 +14227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>972</v>
       </c>
@@ -14280,7 +14268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>976</v>
       </c>
@@ -14321,7 +14309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>980</v>
       </c>
@@ -14362,7 +14350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>984</v>
       </c>
@@ -14403,7 +14391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>988</v>
       </c>
@@ -14444,7 +14432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>992</v>
       </c>
@@ -14485,7 +14473,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>996</v>
       </c>
@@ -14526,7 +14514,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>1000</v>
       </c>
@@ -14567,7 +14555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>1004</v>
       </c>
@@ -14608,7 +14596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>1008</v>
       </c>
@@ -14649,7 +14637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>1012</v>
       </c>
@@ -14690,7 +14678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>1016</v>
       </c>
@@ -14731,7 +14719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>1020</v>
       </c>
@@ -14772,7 +14760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>1024</v>
       </c>
@@ -14813,7 +14801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>1028</v>
       </c>
@@ -14854,7 +14842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>1032</v>
       </c>
@@ -14895,7 +14883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>1036</v>
       </c>
@@ -14936,7 +14924,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>1040</v>
       </c>
@@ -14977,7 +14965,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>1044</v>
       </c>
@@ -15018,7 +15006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>1048</v>
       </c>
@@ -15059,7 +15047,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>1052</v>
       </c>
@@ -15100,7 +15088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>1056</v>
       </c>
@@ -15141,7 +15129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>1060</v>
       </c>
@@ -15182,7 +15170,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>1064</v>
       </c>
@@ -15223,7 +15211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>1068</v>
       </c>
@@ -15264,7 +15252,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>1072</v>
       </c>
@@ -15305,7 +15293,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>1076</v>
       </c>
@@ -15346,7 +15334,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>1080</v>
       </c>
@@ -15387,7 +15375,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>1084</v>
       </c>
@@ -15428,7 +15416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>1088</v>
       </c>
@@ -15469,7 +15457,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>1092</v>
       </c>
@@ -15510,7 +15498,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>1096</v>
       </c>
@@ -15551,7 +15539,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="272" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>1100</v>
       </c>
@@ -15592,7 +15580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>1105</v>
       </c>
@@ -15633,7 +15621,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>1109</v>
       </c>
@@ -15674,7 +15662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>1113</v>
       </c>
@@ -15715,7 +15703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>1117</v>
       </c>
@@ -15756,7 +15744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>1121</v>
       </c>
@@ -15797,7 +15785,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>1125</v>
       </c>
@@ -15838,7 +15826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>1129</v>
       </c>
@@ -15879,7 +15867,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>1133</v>
       </c>
@@ -15920,7 +15908,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>1137</v>
       </c>
@@ -15961,7 +15949,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>1141</v>
       </c>
@@ -16002,7 +15990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>1145</v>
       </c>
@@ -16043,7 +16031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>1149</v>
       </c>
@@ -16084,7 +16072,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>1153</v>
       </c>
@@ -16125,7 +16113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>1157</v>
       </c>
@@ -16166,7 +16154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>1161</v>
       </c>
@@ -16207,7 +16195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>1165</v>
       </c>
@@ -16248,7 +16236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>1169</v>
       </c>
@@ -16289,25 +16277,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="290" spans="1:13" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="291" spans="1:13" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="292" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I292">
         <f>AVERAGE(I2:I289)</f>
         <v>75.757575759517238</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B292" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="EM Resident"/>
-        <filter val="EMT-Basic"/>
-        <filter val="Medical Student"/>
-        <filter val="Paramedic"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:B292" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>